<commit_message>
update on the fetch process
</commit_message>
<xml_diff>
--- a/static/exports/25102020-reporte.xlsx
+++ b/static/exports/25102020-reporte.xlsx
@@ -53,7 +53,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -486,14 +485,10 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Jaro</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Sound</t>
-        </is>
-      </c>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr"/>
       <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Acción</t>
@@ -507,7 +502,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44129.84451388889</v>
+        <v>44129.88555555556</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -531,7 +526,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>asfd</t>
+          <t>no</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -545,7 +540,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>2058</v>
+        <v>90</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -563,7 +558,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44129.84451388889</v>
+        <v>44129.88555555556</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -587,7 +582,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>no</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -601,7 +596,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>775</v>
+        <v>88</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -619,7 +614,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44129.84451388889</v>
+        <v>44129.88555555556</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -643,7 +638,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>no</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -657,7 +652,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>4225</v>
+        <v>85</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>

</xml_diff>